<commit_message>
All files are working
</commit_message>
<xml_diff>
--- a/Bevetel 2017.xlsx
+++ b/Bevetel 2017.xlsx
@@ -5,11 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Bevetelek" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="HelloStreet" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Bartok ter 9A, 15" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Tabor utca 7B 312" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Garazs Rakoczi B71" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Budapesti krt 4b 519" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Osszesites" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="41">
   <si>
     <t xml:space="preserve">Datum</t>
   </si>
@@ -96,9 +100,6 @@
   </si>
   <si>
     <t xml:space="preserve">Osszes bevetel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HelloStreet</t>
   </si>
   <si>
     <t xml:space="preserve">Q1 Bevetel</t>
@@ -202,7 +203,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,7 +213,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9900"/>
-        <bgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
     <fill>
@@ -224,31 +225,55 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE5CD"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9EAD3"/>
-        <bgColor rgb="FFC9DAF8"/>
+        <bgColor rgb="FFD0E0E3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC9DAF8"/>
-        <bgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD0E0E3"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA4C2F4"/>
         <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0E0E3"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF9CB9C"/>
+        <bgColor rgb="FFFFD966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD966"/>
+        <bgColor rgb="FFF9CB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -286,7 +311,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -359,6 +384,58 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -388,8 +465,8 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFCE5CD"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFFFF2CC"/>
+      <rgbColor rgb="FFD0E0E3"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -405,15 +482,15 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFD9EAD3"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFCE5CD"/>
       <rgbColor rgb="FFA4C2F4"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFF9CB9C"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFD966"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -438,10 +515,10 @@
   </sheetPr>
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B113" activeCellId="1" sqref="E2:E54 B113"/>
+      <selection pane="bottomLeft" activeCell="E110" activeCellId="0" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -501,7 +578,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>10500</v>
+        <v>3545</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +663,7 @@
         <v>15</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>8708</v>
+        <v>6545</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,7 +731,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>10366</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -722,7 +799,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>26600</v>
+        <v>6543</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -790,7 +867,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>26850</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,7 +935,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>26600</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -943,7 +1020,7 @@
         <v>12</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>26600</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1028,7 +1105,7 @@
         <v>17</v>
       </c>
       <c r="E34" s="3" t="n">
-        <v>10704</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,7 +1190,7 @@
         <v>17</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>74665</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,7 +1258,7 @@
         <v>15</v>
       </c>
       <c r="E43" s="3" t="n">
-        <v>26850</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,7 +1326,7 @@
         <v>12</v>
       </c>
       <c r="E47" s="3" t="n">
-        <v>26600</v>
+        <v>665</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1300,7 +1377,7 @@
         <v>15</v>
       </c>
       <c r="E50" s="3" t="n">
-        <v>6850</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1368,7 +1445,7 @@
         <v>17</v>
       </c>
       <c r="E54" s="3" t="n">
-        <v>7437</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1453,7 +1530,7 @@
         <v>19</v>
       </c>
       <c r="E59" s="3" t="n">
-        <v>0</v>
+        <v>654</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,7 +1547,7 @@
         <v>19</v>
       </c>
       <c r="E60" s="3" t="n">
-        <v>0</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1521,7 +1598,7 @@
         <v>21</v>
       </c>
       <c r="E63" s="3" t="n">
-        <v>29000</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1589,7 +1666,7 @@
         <v>17</v>
       </c>
       <c r="E67" s="3" t="n">
-        <v>63500</v>
+        <v>654</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,7 +1700,7 @@
         <v>17</v>
       </c>
       <c r="E69" s="3" t="n">
-        <v>7437</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1691,7 +1768,7 @@
         <v>12</v>
       </c>
       <c r="E73" s="3" t="n">
-        <v>30580</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1708,7 +1785,7 @@
         <v>17</v>
       </c>
       <c r="E74" s="3" t="n">
-        <v>56000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1759,7 +1836,7 @@
         <v>15</v>
       </c>
       <c r="E77" s="3" t="n">
-        <v>4000</v>
+        <v>654</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,7 +1887,7 @@
         <v>16</v>
       </c>
       <c r="E80" s="3" t="n">
-        <v>26600</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1955,7 @@
         <v>16</v>
       </c>
       <c r="E84" s="3" t="n">
-        <v>1302</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,7 +1972,7 @@
         <v>16</v>
       </c>
       <c r="E85" s="3" t="n">
-        <v>2117</v>
+        <v>65</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1980,7 +2057,7 @@
         <v>12</v>
       </c>
       <c r="E90" s="3" t="n">
-        <v>26600</v>
+        <v>65</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,7 +2074,7 @@
         <v>17</v>
       </c>
       <c r="E91" s="3" t="n">
-        <v>101000</v>
+        <v>654</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2065,7 +2142,7 @@
         <v>12</v>
       </c>
       <c r="E95" s="3" t="n">
-        <v>0</v>
+        <v>665</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2116,7 +2193,7 @@
         <v>12</v>
       </c>
       <c r="E98" s="3" t="n">
-        <v>0</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2184,7 +2261,7 @@
         <v>12</v>
       </c>
       <c r="E102" s="3" t="n">
-        <v>0</v>
+        <v>654</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,7 +2295,7 @@
         <v>12</v>
       </c>
       <c r="E104" s="3" t="n">
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2269,7 +2346,7 @@
         <v>21</v>
       </c>
       <c r="E107" s="3" t="n">
-        <v>26600</v>
+        <v>6546</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,8 +2427,8 @@
   </sheetPr>
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2:E54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2393,7 +2470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -2401,12 +2478,12 @@
         <f aca="false">SUM(H2:H1000)</f>
         <v>989382</v>
       </c>
-      <c r="D2" s="7" t="str">
+      <c r="D2" s="7" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("FILTER(Bevetelek!A2:E925, Bevetelek!B2:B925 = ""Bartok ter 9A 1/5"")"),"09/01/2017")</f>
-        <v>09/01/2017</v>
+        <v>42744</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>9</v>
@@ -2418,11 +2495,11 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="10" t="str">
+        <v>25</v>
+      </c>
+      <c r="B3" s="10" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &lt;=3))"),"312942")</f>
         <v>312942</v>
       </c>
@@ -2430,7 +2507,7 @@
         <v>42746</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>13</v>
@@ -2442,11 +2519,11 @@
         <v>10467</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="10" t="str">
+        <v>26</v>
+      </c>
+      <c r="B4" s="10" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 3, MONTH(D2:D1000) &lt;= 6))"),"238050")</f>
         <v>238050</v>
       </c>
@@ -2454,7 +2531,7 @@
         <v>42746</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>6</v>
@@ -2466,11 +2543,11 @@
         <v>5688</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="10" t="str">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 6, MONTH(D2:D1000) &lt;= 9))"),"182070")</f>
         <v>182070</v>
       </c>
@@ -2478,7 +2555,7 @@
         <v>42751</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>14</v>
@@ -2490,11 +2567,11 @@
         <v>8708</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="10" t="str">
+        <v>28</v>
+      </c>
+      <c r="B6" s="10" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 9, MONTH(D2:D1000) &lt;= 12))"),"256320")</f>
         <v>256320</v>
       </c>
@@ -2502,7 +2579,7 @@
         <v>42747</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>9</v>
@@ -2514,11 +2591,11 @@
         <v>26570</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="13" t="str">
+        <v>29</v>
+      </c>
+      <c r="B7" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 1))"),"115249")</f>
         <v>115249</v>
       </c>
@@ -2526,7 +2603,7 @@
         <v>42748</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>9</v>
@@ -2538,11 +2615,11 @@
         <v>26850</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="13" t="str">
+        <v>30</v>
+      </c>
+      <c r="B8" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 2))"),"80020")</f>
         <v>80020</v>
       </c>
@@ -2550,7 +2627,7 @@
         <v>42758</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>13</v>
@@ -2562,19 +2639,19 @@
         <v>10366</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="13" t="str">
+        <v>31</v>
+      </c>
+      <c r="B9" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 3))"),"117673")</f>
         <v>117673</v>
       </c>
       <c r="D9" s="14" t="n">
         <v>42776</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>25</v>
+      <c r="E9" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F9" s="15" t="s">
         <v>9</v>
@@ -2586,19 +2663,19 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="13" t="str">
+        <v>32</v>
+      </c>
+      <c r="B10" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 4))"),"80020")</f>
         <v>80020</v>
       </c>
       <c r="D10" s="14" t="n">
         <v>42779</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>25</v>
+      <c r="E10" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F10" s="15" t="s">
         <v>9</v>
@@ -2610,19 +2687,19 @@
         <v>26570</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="13" t="str">
+        <v>33</v>
+      </c>
+      <c r="B11" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 5))"),"98010")</f>
         <v>98010</v>
       </c>
       <c r="D11" s="14" t="n">
         <v>42781</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>25</v>
+      <c r="E11" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F11" s="15" t="s">
         <v>9</v>
@@ -2634,11 +2711,11 @@
         <v>26850</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="13" t="str">
+        <v>34</v>
+      </c>
+      <c r="B12" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 6))"),"60020")</f>
         <v>60020</v>
       </c>
@@ -2646,7 +2723,7 @@
         <v>42802</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>9</v>
@@ -2658,11 +2735,11 @@
         <v>26850</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="13" t="str">
+        <v>35</v>
+      </c>
+      <c r="B13" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 7))"),"42400")</f>
         <v>42400</v>
       </c>
@@ -2670,7 +2747,7 @@
         <v>42801</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>14</v>
@@ -2682,11 +2759,11 @@
         <v>10078</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="13" t="str">
+        <v>36</v>
+      </c>
+      <c r="B14" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 8))"),"44000")</f>
         <v>44000</v>
       </c>
@@ -2694,7 +2771,7 @@
         <v>42796</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>6</v>
@@ -2706,11 +2783,11 @@
         <v>5105</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="13" t="str">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 9))"),"95670")</f>
         <v>95670</v>
       </c>
@@ -2718,7 +2795,7 @@
         <v>42796</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>13</v>
@@ -2730,11 +2807,11 @@
         <v>9958</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="13" t="str">
+        <v>38</v>
+      </c>
+      <c r="B16" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 10))"),"83156")</f>
         <v>83156</v>
       </c>
@@ -2742,7 +2819,7 @@
         <v>42804</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>9</v>
@@ -2754,11 +2831,11 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="13" t="str">
+        <v>39</v>
+      </c>
+      <c r="B17" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 11))"),"93364")</f>
         <v>93364</v>
       </c>
@@ -2766,7 +2843,7 @@
         <v>42811</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>9</v>
@@ -2778,19 +2855,19 @@
         <v>26570</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="13" t="str">
+        <v>40</v>
+      </c>
+      <c r="B18" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 12))"),"79800")</f>
         <v>79800</v>
       </c>
       <c r="D18" s="14" t="n">
         <v>42835</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>25</v>
+      <c r="E18" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F18" s="15" t="s">
         <v>9</v>
@@ -2802,14 +2879,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="13"/>
       <c r="D19" s="14" t="n">
         <v>42836</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>25</v>
+      <c r="E19" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F19" s="15" t="s">
         <v>9</v>
@@ -2821,14 +2898,14 @@
         <v>26570</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="13"/>
       <c r="D20" s="14" t="n">
         <v>42844</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>25</v>
+      <c r="E20" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>9</v>
@@ -2840,14 +2917,14 @@
         <v>26850</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="B21" s="13"/>
       <c r="D21" s="14" t="n">
         <v>42818</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>25</v>
+      <c r="E21" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>13</v>
@@ -2859,14 +2936,14 @@
         <v>12512</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
       <c r="B22" s="13"/>
       <c r="D22" s="11" t="n">
         <v>42857</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>6</v>
@@ -2878,14 +2955,14 @@
         <v>3940</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="13"/>
       <c r="D23" s="11" t="n">
         <v>42857</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>13</v>
@@ -2897,14 +2974,14 @@
         <v>6487</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
       <c r="B24" s="13"/>
       <c r="D24" s="11" t="n">
         <v>42857</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>14</v>
@@ -2916,14 +2993,14 @@
         <v>7563</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4"/>
       <c r="B25" s="13"/>
       <c r="D25" s="11" t="n">
         <v>42863</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>9</v>
@@ -2935,14 +3012,14 @@
         <v>26570</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4"/>
       <c r="B26" s="13"/>
       <c r="D26" s="11" t="n">
         <v>42867</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>9</v>
@@ -2954,14 +3031,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4"/>
       <c r="B27" s="13"/>
       <c r="D27" s="11" t="n">
         <v>42871</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>9</v>
@@ -2973,14 +3050,14 @@
         <v>26850</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4"/>
       <c r="B28" s="13"/>
       <c r="D28" s="14" t="n">
         <v>42898</v>
       </c>
-      <c r="E28" s="8" t="s">
-        <v>25</v>
+      <c r="E28" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F28" s="15" t="s">
         <v>9</v>
@@ -2992,14 +3069,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="13"/>
       <c r="D29" s="14" t="n">
         <v>42899</v>
       </c>
-      <c r="E29" s="8" t="s">
-        <v>25</v>
+      <c r="E29" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F29" s="15" t="s">
         <v>9</v>
@@ -3011,14 +3088,14 @@
         <v>26570</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4"/>
       <c r="B30" s="13"/>
       <c r="D30" s="14" t="n">
         <v>42900</v>
       </c>
-      <c r="E30" s="8" t="s">
-        <v>25</v>
+      <c r="E30" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F30" s="15" t="s">
         <v>9</v>
@@ -3030,14 +3107,14 @@
         <v>6850</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4"/>
       <c r="B31" s="13"/>
       <c r="D31" s="11" t="n">
         <v>42926</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F31" s="8" t="s">
         <v>9</v>
@@ -3049,14 +3126,14 @@
         <v>13400</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4"/>
       <c r="B32" s="13"/>
       <c r="D32" s="11" t="n">
         <v>42934</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F32" s="8" t="s">
         <v>20</v>
@@ -3068,14 +3145,14 @@
         <v>29000</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4"/>
       <c r="B33" s="13"/>
       <c r="D33" s="14" t="n">
         <v>42954</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>25</v>
+      <c r="E33" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F33" s="15" t="s">
         <v>9</v>
@@ -3087,14 +3164,14 @@
         <v>13400</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4"/>
       <c r="B34" s="13"/>
       <c r="D34" s="14" t="n">
         <v>42956</v>
       </c>
-      <c r="E34" s="8" t="s">
-        <v>25</v>
+      <c r="E34" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F34" s="15" t="s">
         <v>9</v>
@@ -3106,14 +3183,14 @@
         <v>13300</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4"/>
       <c r="B35" s="13"/>
       <c r="D35" s="14" t="n">
         <v>42969</v>
       </c>
-      <c r="E35" s="8" t="s">
-        <v>25</v>
+      <c r="E35" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>9</v>
@@ -3125,14 +3202,14 @@
         <v>17300</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4"/>
       <c r="B36" s="13"/>
       <c r="D36" s="11" t="n">
         <v>42982</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F36" s="8" t="s">
         <v>6</v>
@@ -3144,14 +3221,14 @@
         <v>3940</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4"/>
       <c r="B37" s="13"/>
       <c r="D37" s="11" t="n">
         <v>42989</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F37" s="8" t="s">
         <v>9</v>
@@ -3163,14 +3240,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4"/>
       <c r="B38" s="13"/>
       <c r="D38" s="11" t="n">
         <v>42989</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F38" s="8" t="s">
         <v>9</v>
@@ -3182,14 +3259,14 @@
         <v>30550</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4"/>
       <c r="B39" s="13"/>
       <c r="D39" s="11" t="n">
         <v>42989</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F39" s="8" t="s">
         <v>9</v>
@@ -3201,14 +3278,14 @@
         <v>30580</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4"/>
       <c r="B40" s="13"/>
       <c r="D40" s="11" t="n">
         <v>42997</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F40" s="8" t="s">
         <v>14</v>
@@ -3220,14 +3297,14 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4"/>
       <c r="B41" s="13"/>
       <c r="D41" s="14" t="n">
         <v>43017</v>
       </c>
-      <c r="E41" s="8" t="s">
-        <v>25</v>
+      <c r="E41" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F41" s="15" t="s">
         <v>13</v>
@@ -3239,14 +3316,14 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4"/>
       <c r="B42" s="13"/>
       <c r="D42" s="14" t="n">
         <v>43018</v>
       </c>
-      <c r="E42" s="8" t="s">
-        <v>25</v>
+      <c r="E42" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F42" s="15" t="s">
         <v>9</v>
@@ -3258,14 +3335,14 @@
         <v>24655</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4"/>
       <c r="B43" s="13"/>
       <c r="D43" s="14" t="n">
         <v>43019</v>
       </c>
-      <c r="E43" s="8" t="s">
-        <v>25</v>
+      <c r="E43" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>9</v>
@@ -3277,14 +3354,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4"/>
       <c r="B44" s="13"/>
       <c r="D44" s="14" t="n">
         <v>43021</v>
       </c>
-      <c r="E44" s="8" t="s">
-        <v>25</v>
+      <c r="E44" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F44" s="15" t="s">
         <v>9</v>
@@ -3296,14 +3373,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4"/>
       <c r="B45" s="13"/>
       <c r="D45" s="14" t="n">
         <v>43036</v>
       </c>
-      <c r="E45" s="8" t="s">
-        <v>25</v>
+      <c r="E45" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F45" s="15" t="s">
         <v>13</v>
@@ -3315,14 +3392,14 @@
         <v>1302</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4"/>
       <c r="B46" s="13"/>
       <c r="D46" s="14" t="n">
         <v>43036</v>
       </c>
-      <c r="E46" s="8" t="s">
-        <v>25</v>
+      <c r="E46" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="F46" s="15" t="s">
         <v>6</v>
@@ -3334,14 +3411,14 @@
         <v>2117</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4"/>
       <c r="B47" s="13"/>
       <c r="D47" s="11" t="n">
         <v>43045</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F47" s="8" t="s">
         <v>9</v>
@@ -3353,14 +3430,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4"/>
       <c r="B48" s="13"/>
       <c r="D48" s="11" t="n">
         <v>43052</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F48" s="8" t="s">
         <v>9</v>
@@ -3372,14 +3449,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4"/>
       <c r="B49" s="13"/>
       <c r="D49" s="11" t="n">
         <v>43053</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F49" s="8" t="s">
         <v>9</v>
@@ -3391,14 +3468,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4"/>
       <c r="B50" s="13"/>
       <c r="D50" s="11" t="n">
         <v>43059</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F50" s="8" t="s">
         <v>14</v>
@@ -3410,14 +3487,14 @@
         <v>7298</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4"/>
       <c r="B51" s="13"/>
       <c r="D51" s="11" t="n">
         <v>43066</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="F51" s="8" t="s">
         <v>13</v>
@@ -3429,14 +3506,14 @@
         <v>6266</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4"/>
       <c r="B52" s="13"/>
       <c r="D52" s="16" t="n">
         <v>43077</v>
       </c>
-      <c r="E52" s="8" t="s">
-        <v>25</v>
+      <c r="E52" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="F52" s="17" t="s">
         <v>9</v>
@@ -3448,14 +3525,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4"/>
       <c r="B53" s="13"/>
       <c r="D53" s="16" t="n">
         <v>43080</v>
       </c>
-      <c r="E53" s="8" t="s">
-        <v>25</v>
+      <c r="E53" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="F53" s="17" t="s">
         <v>9</v>
@@ -3467,14 +3544,14 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4"/>
       <c r="B54" s="13"/>
       <c r="D54" s="16" t="n">
         <v>43083</v>
       </c>
-      <c r="E54" s="8" t="s">
-        <v>25</v>
+      <c r="E54" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="F54" s="17" t="s">
         <v>9</v>
@@ -3484,6 +3561,1829 @@
       </c>
       <c r="H54" s="17" t="n">
         <v>26600</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I33"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.9030612244898"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <f aca="false">SUM(H2:H1000)</f>
+        <v>1329564</v>
+      </c>
+      <c r="D2" s="18" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("FILTER(Bevetelek!A2:E925, Bevetelek!B2:B925 = ""Tabor utca 7B 3/12"")"),"02/01/2017")</f>
+        <v>42737</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="19" t="n">
+        <v>8604</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &lt;=3))"),"375283")</f>
+        <v>375283</v>
+      </c>
+      <c r="D3" s="20" t="n">
+        <v>42744</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="19" t="n">
+        <v>111000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 3, MONTH(D2:D1000) &lt;= 6))"),"372453")</f>
+        <v>372453</v>
+      </c>
+      <c r="D4" s="20" t="n">
+        <v>42751</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="19" t="n">
+        <v>28757</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 6, MONTH(D2:D1000) &lt;= 9))"),"252136")</f>
+        <v>252136</v>
+      </c>
+      <c r="D5" s="21" t="n">
+        <v>42774</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="22" t="n">
+        <v>101000</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 9, MONTH(D2:D1000) &lt;= 12))"),"329692")</f>
+        <v>329692</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>42774</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="22" t="n">
+        <v>8650</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 1))"),"148361")</f>
+        <v>148361</v>
+      </c>
+      <c r="D7" s="23" t="n">
+        <v>42808</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="24" t="n">
+        <v>111000</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 2))"),"109650")</f>
+        <v>109650</v>
+      </c>
+      <c r="D8" s="25" t="n">
+        <v>42795</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="26" t="n">
+        <v>6272</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 3))"),"117272")</f>
+        <v>117272</v>
+      </c>
+      <c r="D9" s="25" t="n">
+        <v>42838</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="26" t="n">
+        <v>101000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 4))"),"111704")</f>
+        <v>111704</v>
+      </c>
+      <c r="D10" s="27" t="n">
+        <v>42852</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="28" t="n">
+        <v>10704</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 5))"),"149020")</f>
+        <v>149020</v>
+      </c>
+      <c r="D11" s="27" t="n">
+        <v>42861</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="28" t="n">
+        <v>74665</v>
+      </c>
+      <c r="I11" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 6))"),"111729")</f>
+        <v>111729</v>
+      </c>
+      <c r="D12" s="27" t="n">
+        <v>42863</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="28" t="n">
+        <v>8020</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 7))"),"70937")</f>
+        <v>70937</v>
+      </c>
+      <c r="D13" s="27" t="n">
+        <v>42872</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="28" t="n">
+        <v>22670</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 8))"),"72762")</f>
+        <v>72762</v>
+      </c>
+      <c r="D14" s="27" t="n">
+        <v>42872</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="28" t="n">
+        <v>43665</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 9))"),"108437")</f>
+        <v>108437</v>
+      </c>
+      <c r="D15" s="29" t="n">
+        <v>42899</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="30" t="n">
+        <v>6999</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 10))"),"108333")</f>
+        <v>108333</v>
+      </c>
+      <c r="D16" s="29" t="n">
+        <v>42901</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="30" t="n">
+        <v>101000</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 11))"),"108337")</f>
+        <v>108337</v>
+      </c>
+      <c r="D17" s="29" t="n">
+        <v>42913</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="30" t="n">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 12))"),"113022")</f>
+        <v>113022</v>
+      </c>
+      <c r="D18" s="27" t="n">
+        <v>42923</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="28" t="n">
+        <v>7437</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="13"/>
+      <c r="D19" s="27" t="n">
+        <v>42928</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="28" t="n">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="13"/>
+      <c r="D20" s="27" t="n">
+        <v>42929</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="28" t="n">
+        <v>33500</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+      <c r="B21" s="13"/>
+      <c r="D21" s="11" t="n">
+        <v>42956</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="8" t="n">
+        <v>9262</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="13"/>
+      <c r="D22" s="11" t="n">
+        <v>42962</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="8" t="n">
+        <v>63500</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="13"/>
+      <c r="D23" s="21" t="n">
+        <v>42982</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="22" t="n">
+        <v>7437</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4"/>
+      <c r="B24" s="13"/>
+      <c r="D24" s="21" t="n">
+        <v>42993</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="22" t="n">
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+      <c r="B25" s="13"/>
+      <c r="D25" s="21" t="n">
+        <v>42996</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="22" t="n">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+      <c r="B26" s="13"/>
+      <c r="D26" s="21" t="n">
+        <v>42996</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="22" t="n">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+      <c r="B27" s="13"/>
+      <c r="D27" s="11" t="n">
+        <v>43018</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="8" t="n">
+        <v>7333</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="13"/>
+      <c r="D28" s="11" t="n">
+        <v>43025</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H28" s="8" t="n">
+        <v>101000</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="4"/>
+      <c r="B29" s="13"/>
+      <c r="D29" s="21" t="n">
+        <v>43046</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="4"/>
+      <c r="B30" s="13"/>
+      <c r="D30" s="21" t="n">
+        <v>43046</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="22" t="n">
+        <v>7337</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="4"/>
+      <c r="B31" s="13"/>
+      <c r="D31" s="21" t="n">
+        <v>43053</v>
+      </c>
+      <c r="E31" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="22" t="n">
+        <v>101000</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4"/>
+      <c r="B32" s="13"/>
+      <c r="D32" s="11" t="n">
+        <v>43084</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="8" t="n">
+        <v>12022</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="4"/>
+      <c r="B33" s="13"/>
+      <c r="D33" s="11" t="n">
+        <v>43084</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="8" t="n">
+        <v>101000</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="13.9030612244898"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <f aca="false">SUM(H2:H1000)</f>
+        <v>123000</v>
+      </c>
+      <c r="D2" s="7" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("FILTER(Bevetelek!A2:E925, Bevetelek!B2:B925 = ""Rakoczi ut 105 B71 garazs"")"),"05/01/2017")</f>
+        <v>42740</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="8" t="n">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &lt;=3))"),"31500")</f>
+        <v>31500</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>42772</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="8" t="n">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 3, MONTH(D2:D1000) &lt;= 6))"),"31500")</f>
+        <v>31500</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>42797</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="8" t="n">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 6, MONTH(D2:D1000) &lt;= 9))"),"60000")</f>
+        <v>60000</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>42828</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="8" t="n">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 9, MONTH(D2:D1000) &lt;= 12))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>42858</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="8" t="n">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 1))"),"10500")</f>
+        <v>10500</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>42887</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 2))"),"10500")</f>
+        <v>10500</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>42933</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="8" t="n">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 3))"),"10500")</f>
+        <v>10500</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>42964</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 4))"),"10500")</f>
+        <v>10500</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>42995</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 5))"),"10500")</f>
+        <v>10500</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>43025</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 6))"),"10500")</f>
+        <v>10500</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>43056</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 7))"),"60000")</f>
+        <v>60000</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>43086</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 8))"),"0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 9))"),"0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 10))"),"0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 11))"),"0")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 12))"),"0")</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H28"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.9030612244898"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <f aca="false">SUM(H2:H1000)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="18" t="str">
+        <f aca="false">IFERROR(__xludf.dummyfunction("FILTER(Bevetelek!A2:E925, Bevetelek!B2:B925 = ""Budapesti krt 4b 5/19"")"),"15/01/2017")</f>
+        <v>15/01/2017</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &lt;=3))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="20" t="n">
+        <v>42767</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 3, MONTH(D2:D1000) &lt;= 6))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="20" t="n">
+        <v>42795</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 6, MONTH(D2:D1000) &lt;= 9))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="21" t="n">
+        <v>42826</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="10" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) &gt; 9, MONTH(D2:D1000) &lt;= 12))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="21" t="n">
+        <v>42856</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 1))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D7" s="23" t="n">
+        <v>42887</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 2))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="25" t="n">
+        <v>42917</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 3))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="25" t="n">
+        <v>42948</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 4))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="27" t="n">
+        <v>42979</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 5))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="27" t="n">
+        <v>43009</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 6))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="27" t="n">
+        <v>43040</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 7))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 8))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 9))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 10))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 11))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="13" t="n">
+        <f aca="false">IFERROR(__xludf.dummyfunction("SUM(FILTER(H2:H1000, MONTH(D2:D1000) = 12))"),"0")</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4"/>
+      <c r="B19" s="13"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="13"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+      <c r="B21" s="13"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="13"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4"/>
+      <c r="B23" s="13"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4"/>
+      <c r="B24" s="13"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4"/>
+      <c r="B25" s="13"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4"/>
+      <c r="B26" s="13"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4"/>
+      <c r="B27" s="13"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="13"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.9030612244898"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B2+'Tabor utca 7B 312'!B2 + 'Garazs Rakoczi B71'!B2+'Budapesti krt 4b 519'!B2)</f>
+        <v>2441946</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B3+'Tabor utca 7B 312'!B3 + 'Garazs Rakoczi B71'!B3+'Budapesti krt 4b 519'!B3)</f>
+        <v>719725</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B4+'Tabor utca 7B 312'!B4 + 'Garazs Rakoczi B71'!B4+'Budapesti krt 4b 519'!B4)</f>
+        <v>642003</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B5+'Tabor utca 7B 312'!B5 + 'Garazs Rakoczi B71'!B5+'Budapesti krt 4b 519'!B5)</f>
+        <v>494206</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B6+'Tabor utca 7B 312'!B6 + 'Garazs Rakoczi B71'!B6+'Budapesti krt 4b 519'!B6)</f>
+        <v>586012</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B7+'Tabor utca 7B 312'!B7 + 'Garazs Rakoczi B71'!B7+'Budapesti krt 4b 519'!B7)</f>
+        <v>274110</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B8+'Tabor utca 7B 312'!B8 + 'Garazs Rakoczi B71'!B8+'Budapesti krt 4b 519'!B8)</f>
+        <v>200170</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B9+'Tabor utca 7B 312'!B9 + 'Garazs Rakoczi B71'!B9+'Budapesti krt 4b 519'!B9)</f>
+        <v>245445</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B10+'Tabor utca 7B 312'!B10 + 'Garazs Rakoczi B71'!B10+'Budapesti krt 4b 519'!B10)</f>
+        <v>202224</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B11+'Tabor utca 7B 312'!B11 + 'Garazs Rakoczi B71'!B11+'Budapesti krt 4b 519'!B11)</f>
+        <v>257530</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B12+'Tabor utca 7B 312'!B12 + 'Garazs Rakoczi B71'!B12+'Budapesti krt 4b 519'!B12)</f>
+        <v>182249</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B13+'Tabor utca 7B 312'!B13 + 'Garazs Rakoczi B71'!B13+'Budapesti krt 4b 519'!B13)</f>
+        <v>173337</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B14+'Tabor utca 7B 312'!B14 + 'Garazs Rakoczi B71'!B14+'Budapesti krt 4b 519'!B14)</f>
+        <v>116762</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B15+'Tabor utca 7B 312'!B15 + 'Garazs Rakoczi B71'!B15+'Budapesti krt 4b 519'!B15)</f>
+        <v>204107</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B16+'Tabor utca 7B 312'!B16 + 'Garazs Rakoczi B71'!B16+'Budapesti krt 4b 519'!B16)</f>
+        <v>191489</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B17+'Tabor utca 7B 312'!B17 + 'Garazs Rakoczi B71'!B17+'Budapesti krt 4b 519'!B17)</f>
+        <v>201701</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="6" t="n">
+        <f aca="false">SUM('Bartok ter 9A, 15'!B18+'Tabor utca 7B 312'!B18 + 'Garazs Rakoczi B71'!B18+'Budapesti krt 4b 519'!B18)</f>
+        <v>192822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>